<commit_message>
nha sach chuan + mau menu
</commit_message>
<xml_diff>
--- a/data/DataBase/Nhap_Hang.xlsx
+++ b/data/DataBase/Nhap_Hang.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="8520"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="8520" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Dụng cụ học sinh" sheetId="6" r:id="rId1"/>
+    <sheet name="d" sheetId="6" r:id="rId1"/>
     <sheet name="Văn phòng phẩm" sheetId="2" r:id="rId2"/>
     <sheet name="Thiết bị trường học" sheetId="3" r:id="rId3"/>
     <sheet name="Sách giáo khoa" sheetId="4" r:id="rId4"/>
@@ -555,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -791,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>